<commit_message>
pre fixing the memory error
</commit_message>
<xml_diff>
--- a/dfa_sample.xlsx
+++ b/dfa_sample.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,6 +518,420 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>q1</t>
+        </is>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>q1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>q1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>q1</t>
+        </is>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>q1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>q1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>q1</t>
+        </is>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>q1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>q1</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>q0</t>
+        </is>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>q2</t>
+        </is>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
removed re-enter words if doesn't belong to dictionary
</commit_message>
<xml_diff>
--- a/dfa_sample.xlsx
+++ b/dfa_sample.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,420 +518,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>q1</t>
-        </is>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>q1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>q1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="D13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>q1</t>
-        </is>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>q1</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>q1</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="D17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="D18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="D19" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>q1</t>
-        </is>
-      </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>q1</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="D22" t="b">
-        <v>0</v>
-      </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>q1</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>q0</t>
-        </is>
-      </c>
-      <c r="D23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="D24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="D25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>